<commit_message>
17th day - KMEANS clustering finished on clustering_country file Need to do it on the covid19_graph to find clusters relying on covid-19 numbers Need to compare groups
</commit_message>
<xml_diff>
--- a/team9/files/Datasets/dataset_final_2.xlsx
+++ b/team9/files/Datasets/dataset_final_2.xlsx
@@ -449,10 +449,8 @@
       <c r="J2">
         <v>550</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K2">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -490,10 +488,8 @@
       <c r="J3">
         <v>3370</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K3">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -531,10 +527,8 @@
       <c r="J4">
         <v>4860</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K4">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -572,10 +566,8 @@
       <c r="J5">
         <v>40880</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K5">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -613,10 +605,8 @@
       <c r="J6">
         <v>12390</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K6">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -654,10 +644,8 @@
       <c r="J7">
         <v>4230</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K7">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -695,10 +683,8 @@
       <c r="J8">
         <v>53230</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K8">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -736,10 +722,8 @@
       <c r="J9">
         <v>49310</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K9">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -777,10 +761,8 @@
       <c r="J10">
         <v>4050</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K10">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -818,10 +800,8 @@
       <c r="J11">
         <v>280</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K11">
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -859,10 +839,8 @@
       <c r="J12">
         <v>45910</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K12">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -900,10 +878,8 @@
       <c r="J13">
         <v>870</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K13">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -941,10 +917,8 @@
       <c r="J14">
         <v>670</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K14">
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -982,10 +956,8 @@
       <c r="J15">
         <v>1750</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K15">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -1023,10 +995,8 @@
       <c r="J16">
         <v>8860</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K16">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1064,10 +1034,8 @@
       <c r="J17">
         <v>21890</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K17">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1105,10 +1073,8 @@
       <c r="J18">
         <v>5740</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K18">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1146,10 +1112,8 @@
       <c r="J19">
         <v>5670</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K19">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1187,10 +1151,8 @@
       <c r="J20">
         <v>3370</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K20">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1228,10 +1190,8 @@
       <c r="J21">
         <v>9140</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K21">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -1269,10 +1229,8 @@
       <c r="J22">
         <v>2970</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K22">
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -1310,10 +1268,8 @@
       <c r="J23">
         <v>7750</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K23">
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1351,10 +1307,8 @@
       <c r="J24">
         <v>490</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K24">
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1392,10 +1346,8 @@
       <c r="J25">
         <v>44940</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K25">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1433,10 +1385,8 @@
       <c r="J26">
         <v>84410</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K26">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1474,10 +1424,8 @@
       <c r="J27">
         <v>14670</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K27">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1515,10 +1463,8 @@
       <c r="J28">
         <v>9460</v>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K28">
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1556,10 +1502,8 @@
       <c r="J29">
         <v>1600</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K29">
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1597,10 +1541,8 @@
       <c r="J30">
         <v>1440</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K30">
+        <v>3</v>
       </c>
     </row>
     <row r="31">
@@ -1638,10 +1580,8 @@
       <c r="J31">
         <v>1640</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K31">
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1679,10 +1619,8 @@
       <c r="J32">
         <v>6180</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K32">
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1720,10 +1658,8 @@
       <c r="J33">
         <v>1380</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K33">
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -1761,10 +1697,8 @@
       <c r="J34">
         <v>3420</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K34">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1802,10 +1736,8 @@
       <c r="J35">
         <v>11520</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K35">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1843,10 +1775,8 @@
       <c r="J36">
         <v>28570</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K36">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1884,10 +1814,8 @@
       <c r="J37">
         <v>20240</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K37">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1925,10 +1853,8 @@
       <c r="J38">
         <v>47090</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K38">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1966,10 +1892,8 @@
       <c r="J39">
         <v>3190</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K39">
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -2007,10 +1931,8 @@
       <c r="J40">
         <v>60140</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K40">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -2048,10 +1970,8 @@
       <c r="J41">
         <v>7760</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K41">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -2089,10 +2009,8 @@
       <c r="J42">
         <v>6110</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K42">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -2130,10 +2048,8 @@
       <c r="J43">
         <v>2800</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K43">
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -2171,10 +2087,8 @@
       <c r="J44">
         <v>29340</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K44">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -2212,10 +2126,8 @@
       <c r="J45">
         <v>21140</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K45">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2253,10 +2165,8 @@
       <c r="J46">
         <v>790</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K46">
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -2294,10 +2204,8 @@
       <c r="J47">
         <v>48280</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K47">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -2335,10 +2243,8 @@
       <c r="J48">
         <v>41080</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K48">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2376,10 +2282,8 @@
       <c r="J49">
         <v>6830</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K49">
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -2417,10 +2321,8 @@
       <c r="J50">
         <v>41770</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K50">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -2458,10 +2360,8 @@
       <c r="J51">
         <v>4440</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K51">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -2499,10 +2399,8 @@
       <c r="J52">
         <v>2130</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K52">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
@@ -2540,10 +2438,8 @@
       <c r="J53">
         <v>850</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K53">
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -2581,10 +2477,8 @@
       <c r="J54">
         <v>710</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K54">
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -2622,10 +2516,8 @@
       <c r="J55">
         <v>750</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K55">
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -2663,10 +2555,8 @@
       <c r="J56">
         <v>6840</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K56">
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -2704,10 +2594,8 @@
       <c r="J57">
         <v>19770</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K57">
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2745,10 +2633,8 @@
       <c r="J58">
         <v>4400</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K58">
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2786,10 +2672,8 @@
       <c r="J59">
         <v>4770</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K59">
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2827,10 +2711,8 @@
       <c r="J60">
         <v>2350</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K60">
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -2868,10 +2750,8 @@
       <c r="J61">
         <v>14000</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K61">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2909,10 +2789,8 @@
       <c r="J62">
         <v>800</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K62">
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -2950,10 +2828,8 @@
       <c r="J63">
         <v>14780</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K63">
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2991,10 +2867,8 @@
       <c r="J64">
         <v>3840</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K64">
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -3032,10 +2906,8 @@
       <c r="J65">
         <v>2020</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K65">
+        <v>3</v>
       </c>
     </row>
     <row r="66">
@@ -3073,10 +2945,8 @@
       <c r="J66">
         <v>61390</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K66">
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -3114,10 +2984,8 @@
       <c r="J67">
         <v>5040</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K67">
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -3155,10 +3023,8 @@
       <c r="J68">
         <v>67960</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K68">
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -3196,10 +3062,8 @@
       <c r="J69">
         <v>40920</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K69">
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -3237,10 +3101,8 @@
       <c r="J70">
         <v>33730</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K70">
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -3278,10 +3140,8 @@
       <c r="J71">
         <v>4970</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K71">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -3319,10 +3179,8 @@
       <c r="J72">
         <v>4200</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K72">
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -3360,10 +3218,8 @@
       <c r="J73">
         <v>41310</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K73">
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3401,10 +3257,8 @@
       <c r="J74">
         <v>8070</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K74">
+        <v>2</v>
       </c>
     </row>
     <row r="75">
@@ -3442,10 +3296,8 @@
       <c r="J75">
         <v>1620</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K75">
+        <v>3</v>
       </c>
     </row>
     <row r="76">
@@ -3483,10 +3335,8 @@
       <c r="J76">
         <v>1220</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K76">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3524,10 +3374,8 @@
       <c r="J77">
         <v>1390</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K77">
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -3565,10 +3413,8 @@
       <c r="J78">
         <v>30600</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K78">
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -3606,10 +3452,8 @@
       <c r="J79">
         <v>34290</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K79">
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -3647,10 +3491,8 @@
       <c r="J80">
         <v>2450</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K80">
+        <v>3</v>
       </c>
     </row>
     <row r="81">
@@ -3688,10 +3530,8 @@
       <c r="J81">
         <v>7920</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K81">
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -3729,10 +3569,8 @@
       <c r="J82">
         <v>610</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K82">
+        <v>3</v>
       </c>
     </row>
     <row r="83">
@@ -3770,10 +3608,8 @@
       <c r="J83">
         <v>6400</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K83">
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -3811,10 +3647,8 @@
       <c r="J84">
         <v>4060</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K84">
+        <v>2</v>
       </c>
     </row>
     <row r="85">
@@ -3852,10 +3686,8 @@
       <c r="J85">
         <v>17430</v>
       </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K85">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -3893,10 +3725,8 @@
       <c r="J86">
         <v>70870</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K86">
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -3934,10 +3764,8 @@
       <c r="J87">
         <v>16510</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K87">
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -3975,10 +3803,8 @@
       <c r="J88">
         <v>3090</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K88">
+        <v>2</v>
       </c>
     </row>
     <row r="89">
@@ -4016,10 +3842,8 @@
       <c r="J89">
         <v>2980</v>
       </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K89">
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -4057,10 +3881,8 @@
       <c r="J90">
         <v>510</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K90">
+        <v>3</v>
       </c>
     </row>
     <row r="91">
@@ -4098,10 +3920,8 @@
       <c r="J91">
         <v>9180</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K91">
+        <v>2</v>
       </c>
     </row>
     <row r="92">
@@ -4139,10 +3959,8 @@
       <c r="J92">
         <v>5450</v>
       </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K92">
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -4180,10 +3998,8 @@
       <c r="J93">
         <v>840</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K93">
+        <v>3</v>
       </c>
     </row>
     <row r="94">
@@ -4221,10 +4037,8 @@
       <c r="J94">
         <v>1310</v>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K94">
+        <v>3</v>
       </c>
     </row>
     <row r="95">
@@ -4262,10 +4076,8 @@
       <c r="J95">
         <v>3660</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K95">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -4303,10 +4115,8 @@
       <c r="J96">
         <v>460</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K96">
+        <v>3</v>
       </c>
     </row>
     <row r="97">
@@ -4344,10 +4154,8 @@
       <c r="J97">
         <v>1160</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K97">
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -4385,10 +4193,8 @@
       <c r="J98">
         <v>12050</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K98">
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -4426,10 +4232,8 @@
       <c r="J99">
         <v>360</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K99">
+        <v>3</v>
       </c>
     </row>
     <row r="100">
@@ -4467,10 +4271,8 @@
       <c r="J100">
         <v>10590</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K100">
+        <v>2</v>
       </c>
     </row>
     <row r="101">
@@ -4508,10 +4310,8 @@
       <c r="J101">
         <v>5220</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K101">
+        <v>3</v>
       </c>
     </row>
     <row r="102">
@@ -4549,10 +4349,8 @@
       <c r="J102">
         <v>390</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K102">
+        <v>3</v>
       </c>
     </row>
     <row r="103">
@@ -4590,10 +4388,8 @@
       <c r="J103">
         <v>1960</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K103">
+        <v>3</v>
       </c>
     </row>
     <row r="104">
@@ -4631,10 +4427,8 @@
       <c r="J104">
         <v>2030</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K104">
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -4672,10 +4466,8 @@
       <c r="J105">
         <v>51260</v>
       </c>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K105">
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -4713,10 +4505,8 @@
       <c r="J106">
         <v>80610</v>
       </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K106">
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -4754,10 +4544,8 @@
       <c r="J107">
         <v>970</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K107">
+        <v>3</v>
       </c>
     </row>
     <row r="108">
@@ -4795,10 +4583,8 @@
       <c r="J108">
         <v>40640</v>
       </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K108">
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -4836,10 +4622,8 @@
       <c r="J109">
         <v>15140</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K109">
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -4877,10 +4661,8 @@
       <c r="J110">
         <v>1590</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K110">
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -4918,10 +4700,8 @@
       <c r="J111">
         <v>14370</v>
       </c>
-      <c r="K111" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K111">
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -4959,10 +4739,8 @@
       <c r="J112">
         <v>6470</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K112">
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -5000,10 +4778,8 @@
       <c r="J113">
         <v>3830</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K113">
+        <v>2</v>
       </c>
     </row>
     <row r="114">
@@ -5041,10 +4817,8 @@
       <c r="J114">
         <v>2570</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K114">
+        <v>3</v>
       </c>
     </row>
     <row r="115">
@@ -5082,10 +4856,8 @@
       <c r="J115">
         <v>14100</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K115">
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -5123,10 +4895,8 @@
       <c r="J116">
         <v>21990</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K116">
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -5164,10 +4934,8 @@
       <c r="J117">
         <v>5670</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K117">
+        <v>2</v>
       </c>
     </row>
     <row r="118">
@@ -5205,10 +4973,8 @@
       <c r="J118">
         <v>61150</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K118">
+        <v>2</v>
       </c>
     </row>
     <row r="119">
@@ -5246,10 +5012,8 @@
       <c r="J119">
         <v>10230</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K119">
+        <v>2</v>
       </c>
     </row>
     <row r="120">
@@ -5287,10 +5051,8 @@
       <c r="J120">
         <v>780</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K120">
+        <v>3</v>
       </c>
     </row>
     <row r="121">
@@ -5328,10 +5090,8 @@
       <c r="J121">
         <v>21600</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K121">
+        <v>2</v>
       </c>
     </row>
     <row r="122">
@@ -5369,10 +5129,8 @@
       <c r="J122">
         <v>1560</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K122">
+        <v>3</v>
       </c>
     </row>
     <row r="123">
@@ -5410,10 +5168,8 @@
       <c r="J123">
         <v>1410</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K123">
+        <v>3</v>
       </c>
     </row>
     <row r="124">
@@ -5451,10 +5207,8 @@
       <c r="J124">
         <v>58770</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K124">
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -5492,10 +5246,8 @@
       <c r="J125">
         <v>490</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K125">
+        <v>3</v>
       </c>
     </row>
     <row r="126">
@@ -5533,10 +5285,8 @@
       <c r="J126">
         <v>3820</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K126">
+        <v>1</v>
       </c>
     </row>
     <row r="127">
@@ -5574,10 +5324,8 @@
       <c r="J127">
         <v>5210</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K127">
+        <v>1</v>
       </c>
     </row>
     <row r="128">
@@ -5615,10 +5363,8 @@
       <c r="J128">
         <v>18260</v>
       </c>
-      <c r="K128" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K128">
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -5656,10 +5402,8 @@
       <c r="J129">
         <v>24580</v>
       </c>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K129">
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -5697,10 +5441,8 @@
       <c r="J130">
         <v>55490</v>
       </c>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K130">
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -5738,10 +5480,8 @@
       <c r="J131">
         <v>3930</v>
       </c>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K131">
+        <v>3</v>
       </c>
     </row>
     <row r="132">
@@ -5779,10 +5519,8 @@
       <c r="J132">
         <v>670</v>
       </c>
-      <c r="K132" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K132">
+        <v>3</v>
       </c>
     </row>
     <row r="133">
@@ -5820,10 +5558,8 @@
       <c r="J133">
         <v>660</v>
       </c>
-      <c r="K133" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K133">
+        <v>3</v>
       </c>
     </row>
     <row r="134">
@@ -5861,10 +5597,8 @@
       <c r="J134">
         <v>6610</v>
       </c>
-      <c r="K134" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K134">
+        <v>2</v>
       </c>
     </row>
     <row r="135">
@@ -5902,10 +5636,8 @@
       <c r="J135">
         <v>1010</v>
       </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K135">
+        <v>2</v>
       </c>
     </row>
     <row r="136">
@@ -5943,10 +5675,8 @@
       <c r="J136">
         <v>15950</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K136">
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -5984,10 +5714,8 @@
       <c r="J137">
         <v>3500</v>
       </c>
-      <c r="K137" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K137">
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -6025,10 +5753,8 @@
       <c r="J138">
         <v>10420</v>
       </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K138">
+        <v>2</v>
       </c>
     </row>
     <row r="139">
@@ -6066,10 +5792,8 @@
       <c r="J139">
         <v>1020</v>
       </c>
-      <c r="K139" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K139">
+        <v>3</v>
       </c>
     </row>
     <row r="140">
@@ -6107,10 +5831,8 @@
       <c r="J140">
         <v>620</v>
       </c>
-      <c r="K140" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K140">
+        <v>3</v>
       </c>
     </row>
     <row r="141">
@@ -6148,10 +5870,8 @@
       <c r="J141">
         <v>2660</v>
       </c>
-      <c r="K141" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K141">
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -6189,10 +5909,8 @@
       <c r="J142">
         <v>15650</v>
       </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="K142">
+        <v>1</v>
       </c>
     </row>
     <row r="143">
@@ -6230,10 +5948,8 @@
       <c r="J143">
         <v>63080</v>
       </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="K143">
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -6271,10 +5987,8 @@
       <c r="J144">
         <v>2020</v>
       </c>
-      <c r="K144" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K144">
+        <v>2</v>
       </c>
     </row>
     <row r="145">
@@ -6312,10 +6026,8 @@
       <c r="J145">
         <v>2360</v>
       </c>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K145">
+        <v>2</v>
       </c>
     </row>
     <row r="146">
@@ -6353,10 +6065,8 @@
       <c r="J146">
         <v>5750</v>
       </c>
-      <c r="K146" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K146">
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -6394,10 +6104,8 @@
       <c r="J147">
         <v>1430</v>
       </c>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K147">
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -6435,10 +6143,8 @@
       <c r="J148">
         <v>1790</v>
       </c>
-      <c r="K148" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="K148">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
second to last push : - After organization of the team 9 folder - Before cleaning the team 9 folder - Before last calculation (average, ... )
</commit_message>
<xml_diff>
--- a/team9/files/Datasets/dataset_final_2.xlsx
+++ b/team9/files/Datasets/dataset_final_2.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K148"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,11 +408,6 @@
           <t>RNB_inhab_year</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Cluster</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -449,9 +444,6 @@
       <c r="J2">
         <v>550</v>
       </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -488,9 +480,6 @@
       <c r="J3">
         <v>3370</v>
       </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -527,9 +516,6 @@
       <c r="J4">
         <v>4860</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -566,9 +552,6 @@
       <c r="J5">
         <v>40880</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -605,9 +588,6 @@
       <c r="J6">
         <v>12390</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -644,9 +624,6 @@
       <c r="J7">
         <v>4230</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -683,9 +660,6 @@
       <c r="J8">
         <v>53230</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -722,9 +696,6 @@
       <c r="J9">
         <v>49310</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -761,9 +732,6 @@
       <c r="J10">
         <v>4050</v>
       </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -800,9 +768,6 @@
       <c r="J11">
         <v>280</v>
       </c>
-      <c r="K11">
-        <v>3</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -839,9 +804,6 @@
       <c r="J12">
         <v>45910</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -878,9 +840,6 @@
       <c r="J13">
         <v>870</v>
       </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -917,9 +876,6 @@
       <c r="J14">
         <v>670</v>
       </c>
-      <c r="K14">
-        <v>3</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -956,9 +912,6 @@
       <c r="J15">
         <v>1750</v>
       </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -995,9 +948,6 @@
       <c r="J16">
         <v>8860</v>
       </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1034,9 +984,6 @@
       <c r="J17">
         <v>21890</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1073,9 +1020,6 @@
       <c r="J18">
         <v>5740</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1112,9 +1056,6 @@
       <c r="J19">
         <v>5670</v>
       </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1151,9 +1092,6 @@
       <c r="J20">
         <v>3370</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1190,9 +1128,6 @@
       <c r="J21">
         <v>9140</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1229,9 +1164,6 @@
       <c r="J22">
         <v>2970</v>
       </c>
-      <c r="K22">
-        <v>3</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1268,9 +1200,6 @@
       <c r="J23">
         <v>7750</v>
       </c>
-      <c r="K23">
-        <v>3</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1307,9 +1236,6 @@
       <c r="J24">
         <v>490</v>
       </c>
-      <c r="K24">
-        <v>3</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1346,9 +1272,6 @@
       <c r="J25">
         <v>44940</v>
       </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1385,9 +1308,6 @@
       <c r="J26">
         <v>84410</v>
       </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1424,9 +1344,6 @@
       <c r="J27">
         <v>14670</v>
       </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1463,9 +1380,6 @@
       <c r="J28">
         <v>9460</v>
       </c>
-      <c r="K28">
-        <v>2</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1502,9 +1416,6 @@
       <c r="J29">
         <v>1600</v>
       </c>
-      <c r="K29">
-        <v>3</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1541,9 +1452,6 @@
       <c r="J30">
         <v>1440</v>
       </c>
-      <c r="K30">
-        <v>3</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1580,9 +1488,6 @@
       <c r="J31">
         <v>1640</v>
       </c>
-      <c r="K31">
-        <v>3</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1619,9 +1524,6 @@
       <c r="J32">
         <v>6180</v>
       </c>
-      <c r="K32">
-        <v>2</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1658,9 +1560,6 @@
       <c r="J33">
         <v>1380</v>
       </c>
-      <c r="K33">
-        <v>3</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1697,9 +1596,6 @@
       <c r="J34">
         <v>3420</v>
       </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1736,9 +1632,6 @@
       <c r="J35">
         <v>11520</v>
       </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1775,9 +1668,6 @@
       <c r="J36">
         <v>28570</v>
       </c>
-      <c r="K36">
-        <v>1</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1814,9 +1704,6 @@
       <c r="J37">
         <v>20240</v>
       </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1853,9 +1740,6 @@
       <c r="J38">
         <v>47090</v>
       </c>
-      <c r="K38">
-        <v>1</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1892,9 +1776,6 @@
       <c r="J39">
         <v>3190</v>
       </c>
-      <c r="K39">
-        <v>3</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1931,9 +1812,6 @@
       <c r="J40">
         <v>60140</v>
       </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1970,9 +1848,6 @@
       <c r="J41">
         <v>7760</v>
       </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2009,9 +1884,6 @@
       <c r="J42">
         <v>6110</v>
       </c>
-      <c r="K42">
-        <v>1</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2048,9 +1920,6 @@
       <c r="J43">
         <v>2800</v>
       </c>
-      <c r="K43">
-        <v>2</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2087,9 +1956,6 @@
       <c r="J44">
         <v>29340</v>
       </c>
-      <c r="K44">
-        <v>1</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2126,9 +1992,6 @@
       <c r="J45">
         <v>21140</v>
       </c>
-      <c r="K45">
-        <v>1</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2165,9 +2028,6 @@
       <c r="J46">
         <v>790</v>
       </c>
-      <c r="K46">
-        <v>3</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2204,9 +2064,6 @@
       <c r="J47">
         <v>48280</v>
       </c>
-      <c r="K47">
-        <v>1</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2243,9 +2100,6 @@
       <c r="J48">
         <v>41080</v>
       </c>
-      <c r="K48">
-        <v>1</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2282,9 +2136,6 @@
       <c r="J49">
         <v>6830</v>
       </c>
-      <c r="K49">
-        <v>3</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2321,9 +2172,6 @@
       <c r="J50">
         <v>41770</v>
       </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2360,9 +2208,6 @@
       <c r="J51">
         <v>4440</v>
       </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2399,9 +2244,6 @@
       <c r="J52">
         <v>2130</v>
       </c>
-      <c r="K52">
-        <v>3</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2438,9 +2280,6 @@
       <c r="J53">
         <v>850</v>
       </c>
-      <c r="K53">
-        <v>3</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2477,9 +2316,6 @@
       <c r="J54">
         <v>710</v>
       </c>
-      <c r="K54">
-        <v>3</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2516,9 +2352,6 @@
       <c r="J55">
         <v>750</v>
       </c>
-      <c r="K55">
-        <v>3</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2555,9 +2388,6 @@
       <c r="J56">
         <v>6840</v>
       </c>
-      <c r="K56">
-        <v>3</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2594,9 +2424,6 @@
       <c r="J57">
         <v>19770</v>
       </c>
-      <c r="K57">
-        <v>1</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2633,9 +2460,6 @@
       <c r="J58">
         <v>4400</v>
       </c>
-      <c r="K58">
-        <v>3</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2672,9 +2496,6 @@
       <c r="J59">
         <v>4770</v>
       </c>
-      <c r="K59">
-        <v>1</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2711,9 +2532,6 @@
       <c r="J60">
         <v>2350</v>
       </c>
-      <c r="K60">
-        <v>3</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2750,9 +2568,6 @@
       <c r="J61">
         <v>14000</v>
       </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2789,9 +2604,6 @@
       <c r="J62">
         <v>800</v>
       </c>
-      <c r="K62">
-        <v>3</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2828,9 +2640,6 @@
       <c r="J63">
         <v>14780</v>
       </c>
-      <c r="K63">
-        <v>1</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2867,9 +2676,6 @@
       <c r="J64">
         <v>3840</v>
       </c>
-      <c r="K64">
-        <v>2</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2906,9 +2712,6 @@
       <c r="J65">
         <v>2020</v>
       </c>
-      <c r="K65">
-        <v>3</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2945,9 +2748,6 @@
       <c r="J66">
         <v>61390</v>
       </c>
-      <c r="K66">
-        <v>1</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2984,9 +2784,6 @@
       <c r="J67">
         <v>5040</v>
       </c>
-      <c r="K67">
-        <v>2</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3023,9 +2820,6 @@
       <c r="J68">
         <v>67960</v>
       </c>
-      <c r="K68">
-        <v>1</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3062,9 +2856,6 @@
       <c r="J69">
         <v>40920</v>
       </c>
-      <c r="K69">
-        <v>1</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3101,9 +2892,6 @@
       <c r="J70">
         <v>33730</v>
       </c>
-      <c r="K70">
-        <v>1</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3140,9 +2928,6 @@
       <c r="J71">
         <v>4970</v>
       </c>
-      <c r="K71">
-        <v>1</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3179,9 +2964,6 @@
       <c r="J72">
         <v>4200</v>
       </c>
-      <c r="K72">
-        <v>2</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3218,9 +3000,6 @@
       <c r="J73">
         <v>41310</v>
       </c>
-      <c r="K73">
-        <v>1</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3257,9 +3036,6 @@
       <c r="J74">
         <v>8070</v>
       </c>
-      <c r="K74">
-        <v>2</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3296,9 +3072,6 @@
       <c r="J75">
         <v>1620</v>
       </c>
-      <c r="K75">
-        <v>3</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3335,9 +3108,6 @@
       <c r="J76">
         <v>1220</v>
       </c>
-      <c r="K76">
-        <v>1</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3374,9 +3144,6 @@
       <c r="J77">
         <v>1390</v>
       </c>
-      <c r="K77">
-        <v>3</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3413,9 +3180,6 @@
       <c r="J78">
         <v>30600</v>
       </c>
-      <c r="K78">
-        <v>1</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3452,9 +3216,6 @@
       <c r="J79">
         <v>34290</v>
       </c>
-      <c r="K79">
-        <v>1</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3491,9 +3252,6 @@
       <c r="J80">
         <v>2450</v>
       </c>
-      <c r="K80">
-        <v>3</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3530,9 +3288,6 @@
       <c r="J81">
         <v>7920</v>
       </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3569,9 +3324,6 @@
       <c r="J82">
         <v>610</v>
       </c>
-      <c r="K82">
-        <v>3</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3608,9 +3360,6 @@
       <c r="J83">
         <v>6400</v>
       </c>
-      <c r="K83">
-        <v>2</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3647,9 +3396,6 @@
       <c r="J84">
         <v>4060</v>
       </c>
-      <c r="K84">
-        <v>2</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3686,9 +3432,6 @@
       <c r="J85">
         <v>17430</v>
       </c>
-      <c r="K85">
-        <v>1</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3725,9 +3468,6 @@
       <c r="J86">
         <v>70870</v>
       </c>
-      <c r="K86">
-        <v>1</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3764,9 +3504,6 @@
       <c r="J87">
         <v>16510</v>
       </c>
-      <c r="K87">
-        <v>1</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3803,9 +3540,6 @@
       <c r="J88">
         <v>3090</v>
       </c>
-      <c r="K88">
-        <v>2</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3842,9 +3576,6 @@
       <c r="J89">
         <v>2980</v>
       </c>
-      <c r="K89">
-        <v>1</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3881,9 +3612,6 @@
       <c r="J90">
         <v>510</v>
       </c>
-      <c r="K90">
-        <v>3</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3920,9 +3648,6 @@
       <c r="J91">
         <v>9180</v>
       </c>
-      <c r="K91">
-        <v>2</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3959,9 +3684,6 @@
       <c r="J92">
         <v>5450</v>
       </c>
-      <c r="K92">
-        <v>1</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3998,9 +3720,6 @@
       <c r="J93">
         <v>840</v>
       </c>
-      <c r="K93">
-        <v>3</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4037,9 +3756,6 @@
       <c r="J94">
         <v>1310</v>
       </c>
-      <c r="K94">
-        <v>3</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4076,9 +3792,6 @@
       <c r="J95">
         <v>3660</v>
       </c>
-      <c r="K95">
-        <v>1</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4115,9 +3828,6 @@
       <c r="J96">
         <v>460</v>
       </c>
-      <c r="K96">
-        <v>3</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4154,9 +3864,6 @@
       <c r="J97">
         <v>1160</v>
       </c>
-      <c r="K97">
-        <v>3</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4193,9 +3900,6 @@
       <c r="J98">
         <v>12050</v>
       </c>
-      <c r="K98">
-        <v>1</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4232,9 +3936,6 @@
       <c r="J99">
         <v>360</v>
       </c>
-      <c r="K99">
-        <v>3</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4271,9 +3972,6 @@
       <c r="J100">
         <v>10590</v>
       </c>
-      <c r="K100">
-        <v>2</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4310,9 +4008,6 @@
       <c r="J101">
         <v>5220</v>
       </c>
-      <c r="K101">
-        <v>3</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4349,9 +4044,6 @@
       <c r="J102">
         <v>390</v>
       </c>
-      <c r="K102">
-        <v>3</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4388,9 +4080,6 @@
       <c r="J103">
         <v>1960</v>
       </c>
-      <c r="K103">
-        <v>3</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4427,9 +4116,6 @@
       <c r="J104">
         <v>2030</v>
       </c>
-      <c r="K104">
-        <v>1</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4466,9 +4152,6 @@
       <c r="J105">
         <v>51260</v>
       </c>
-      <c r="K105">
-        <v>1</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4505,9 +4188,6 @@
       <c r="J106">
         <v>80610</v>
       </c>
-      <c r="K106">
-        <v>1</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4544,9 +4224,6 @@
       <c r="J107">
         <v>970</v>
       </c>
-      <c r="K107">
-        <v>3</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4583,9 +4260,6 @@
       <c r="J108">
         <v>40640</v>
       </c>
-      <c r="K108">
-        <v>1</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4622,9 +4296,6 @@
       <c r="J109">
         <v>15140</v>
       </c>
-      <c r="K109">
-        <v>2</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4661,9 +4332,6 @@
       <c r="J110">
         <v>1590</v>
       </c>
-      <c r="K110">
-        <v>3</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4700,9 +4368,6 @@
       <c r="J111">
         <v>14370</v>
       </c>
-      <c r="K111">
-        <v>1</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4739,9 +4404,6 @@
       <c r="J112">
         <v>6470</v>
       </c>
-      <c r="K112">
-        <v>1</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4778,9 +4440,6 @@
       <c r="J113">
         <v>3830</v>
       </c>
-      <c r="K113">
-        <v>2</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4817,9 +4476,6 @@
       <c r="J114">
         <v>2570</v>
       </c>
-      <c r="K114">
-        <v>3</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4856,9 +4512,6 @@
       <c r="J115">
         <v>14100</v>
       </c>
-      <c r="K115">
-        <v>1</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4895,9 +4548,6 @@
       <c r="J116">
         <v>21990</v>
       </c>
-      <c r="K116">
-        <v>1</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4934,9 +4584,6 @@
       <c r="J117">
         <v>5670</v>
       </c>
-      <c r="K117">
-        <v>2</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4973,9 +4620,6 @@
       <c r="J118">
         <v>61150</v>
       </c>
-      <c r="K118">
-        <v>2</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5012,9 +4656,6 @@
       <c r="J119">
         <v>10230</v>
       </c>
-      <c r="K119">
-        <v>2</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5051,9 +4692,6 @@
       <c r="J120">
         <v>780</v>
       </c>
-      <c r="K120">
-        <v>3</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5090,9 +4728,6 @@
       <c r="J121">
         <v>21600</v>
       </c>
-      <c r="K121">
-        <v>2</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5129,9 +4764,6 @@
       <c r="J122">
         <v>1560</v>
       </c>
-      <c r="K122">
-        <v>3</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5168,9 +4800,6 @@
       <c r="J123">
         <v>1410</v>
       </c>
-      <c r="K123">
-        <v>3</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5207,9 +4836,6 @@
       <c r="J124">
         <v>58770</v>
       </c>
-      <c r="K124">
-        <v>2</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5246,9 +4872,6 @@
       <c r="J125">
         <v>490</v>
       </c>
-      <c r="K125">
-        <v>3</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5285,9 +4908,6 @@
       <c r="J126">
         <v>3820</v>
       </c>
-      <c r="K126">
-        <v>1</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5324,9 +4944,6 @@
       <c r="J127">
         <v>5210</v>
       </c>
-      <c r="K127">
-        <v>1</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5363,9 +4980,6 @@
       <c r="J128">
         <v>18260</v>
       </c>
-      <c r="K128">
-        <v>1</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5402,9 +5016,6 @@
       <c r="J129">
         <v>24580</v>
       </c>
-      <c r="K129">
-        <v>1</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5441,9 +5052,6 @@
       <c r="J130">
         <v>55490</v>
       </c>
-      <c r="K130">
-        <v>1</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5480,9 +5088,6 @@
       <c r="J131">
         <v>3930</v>
       </c>
-      <c r="K131">
-        <v>3</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5519,9 +5124,6 @@
       <c r="J132">
         <v>670</v>
       </c>
-      <c r="K132">
-        <v>3</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5558,9 +5160,6 @@
       <c r="J133">
         <v>660</v>
       </c>
-      <c r="K133">
-        <v>3</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5597,9 +5196,6 @@
       <c r="J134">
         <v>6610</v>
       </c>
-      <c r="K134">
-        <v>2</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5636,9 +5232,6 @@
       <c r="J135">
         <v>1010</v>
       </c>
-      <c r="K135">
-        <v>2</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5675,9 +5268,6 @@
       <c r="J136">
         <v>15950</v>
       </c>
-      <c r="K136">
-        <v>1</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5714,9 +5304,6 @@
       <c r="J137">
         <v>3500</v>
       </c>
-      <c r="K137">
-        <v>1</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5753,9 +5340,6 @@
       <c r="J138">
         <v>10420</v>
       </c>
-      <c r="K138">
-        <v>2</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5792,9 +5376,6 @@
       <c r="J139">
         <v>1020</v>
       </c>
-      <c r="K139">
-        <v>3</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5831,9 +5412,6 @@
       <c r="J140">
         <v>620</v>
       </c>
-      <c r="K140">
-        <v>3</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5870,9 +5448,6 @@
       <c r="J141">
         <v>2660</v>
       </c>
-      <c r="K141">
-        <v>1</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5909,9 +5484,6 @@
       <c r="J142">
         <v>15650</v>
       </c>
-      <c r="K142">
-        <v>1</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5948,9 +5520,6 @@
       <c r="J143">
         <v>63080</v>
       </c>
-      <c r="K143">
-        <v>1</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5987,9 +5556,6 @@
       <c r="J144">
         <v>2020</v>
       </c>
-      <c r="K144">
-        <v>2</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6026,9 +5592,6 @@
       <c r="J145">
         <v>2360</v>
       </c>
-      <c r="K145">
-        <v>2</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -6065,9 +5628,6 @@
       <c r="J146">
         <v>5750</v>
       </c>
-      <c r="K146">
-        <v>1</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -6104,9 +5664,6 @@
       <c r="J147">
         <v>1430</v>
       </c>
-      <c r="K147">
-        <v>3</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -6142,9 +5699,6 @@
       </c>
       <c r="J148">
         <v>1790</v>
-      </c>
-      <c r="K148">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>